<commit_message>
create a document for each client with the correct information (name, account and balance)
</commit_message>
<xml_diff>
--- a/Input/Datos Clientes.xlsx
+++ b/Input/Datos Clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\Documents\Internet Explorer\Universidad\work\PwC\Banco ABC\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B3C94F-893D-4EA4-B517-28513DE8C9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17328817-19E8-4444-83D1-A2B45108B617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16515" yWindow="840" windowWidth="15375" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18555" yWindow="1275" windowWidth="15375" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +120,11 @@
       <color theme="1"/>
       <name val="Segoe UI Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Segoe UI Light"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,6 +163,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -526,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
@@ -1452,6 +1464,11 @@
       <c r="C83" s="5">
         <v>-4117</v>
       </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A95">

</xml_diff>

<commit_message>
now it  sum the account balances and add it to the document
</commit_message>
<xml_diff>
--- a/Input/Datos Clientes.xlsx
+++ b/Input/Datos Clientes.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\Documents\Internet Explorer\Universidad\work\PwC\Banco ABC\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17328817-19E8-4444-83D1-A2B45108B617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A66F60-CC1E-46F5-88D9-58D0F30F0292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18555" yWindow="1275" windowWidth="15375" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>

</xml_diff>